<commit_message>
Updated so that state was ordered
</commit_message>
<xml_diff>
--- a/data-raw/catalog.xlsx
+++ b/data-raw/catalog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaylee/Desktop/cpsvote/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaylee/Desktop/cpsvote/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F170D66A-225A-304E-9F33-549B84B274B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33C4115-6209-0D48-9E22-6DA3BE228921}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="1bbBXZEuvpXUWOM4H2dfSf4qEe/w9aOR03O17HJVfeBciv1kJfxQcX2uJxQ8G/6hB+8cpQEqFL6wwb4yaAP/1w==" workbookSaltValue="po6nkgUJ66gqb2vNNVbSbw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4840" windowWidth="27640" windowHeight="16940" xr2:uid="{F3FFB08B-FE6D-ED48-9525-18B361D5DDB4}"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4409" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4422" uniqueCount="477">
   <si>
     <t>year</t>
   </si>
@@ -1839,7 +1839,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1934,6 +1934,9 @@
       <c r="H3" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I3" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -2267,6 +2270,9 @@
       <c r="H15" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I15" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
@@ -2742,6 +2748,9 @@
       <c r="H32" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I32" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
@@ -3217,6 +3226,9 @@
       <c r="H49" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I49" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
@@ -3692,6 +3704,9 @@
       <c r="H66" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I66" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
@@ -4167,6 +4182,9 @@
       <c r="H83" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I83" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
@@ -4645,6 +4663,9 @@
       <c r="H100" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I100" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
@@ -5120,6 +5141,9 @@
       <c r="H117" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I117" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
@@ -5595,6 +5619,9 @@
       <c r="H134" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I134" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
@@ -6070,6 +6097,9 @@
       <c r="H151" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I151" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
@@ -6545,6 +6575,9 @@
       <c r="H168" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I168" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
@@ -7020,6 +7053,9 @@
       <c r="H185" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="I185" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="3">
@@ -7494,6 +7530,9 @@
       </c>
       <c r="H202" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="I202" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix wrong index in default catalog
</commit_message>
<xml_diff>
--- a/data-raw/catalog.xlsx
+++ b/data-raw/catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaylee/Desktop/cpsvote/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33C4115-6209-0D48-9E22-6DA3BE228921}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7056404-C948-9849-9694-DBDA96837FA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="1bbBXZEuvpXUWOM4H2dfSf4qEe/w9aOR03O17HJVfeBciv1kJfxQcX2uJxQ8G/6hB+8cpQEqFL6wwb4yaAP/1w==" workbookSaltValue="po6nkgUJ66gqb2vNNVbSbw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4840" windowWidth="27640" windowHeight="16940" xr2:uid="{F3FFB08B-FE6D-ED48-9525-18B361D5DDB4}"/>
@@ -1838,8 +1838,8 @@
   <dimension ref="A1:I217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3218,7 +3218,7 @@
         <v>93</v>
       </c>
       <c r="F49" s="3">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Did a dumb thing and forgot to copy the year down to all factors in the catalog
</commit_message>
<xml_diff>
--- a/data-raw/catalog.xlsx
+++ b/data-raw/catalog.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaylee/Desktop/cpsvote/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7056404-C948-9849-9694-DBDA96837FA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB83E937-03BF-734D-9FD5-B38971454BBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="1bbBXZEuvpXUWOM4H2dfSf4qEe/w9aOR03O17HJVfeBciv1kJfxQcX2uJxQ8G/6hB+8cpQEqFL6wwb4yaAP/1w==" workbookSaltValue="po6nkgUJ66gqb2vNNVbSbw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="4840" windowWidth="27640" windowHeight="16940" xr2:uid="{F3FFB08B-FE6D-ED48-9525-18B361D5DDB4}"/>
+    <workbookView xWindow="1500" yWindow="4840" windowWidth="27640" windowHeight="16940" activeTab="11" xr2:uid="{F3FFB08B-FE6D-ED48-9525-18B361D5DDB4}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -1837,7 +1837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFB3A44-3E53-2642-A3DE-5CB8717D98DA}">
   <dimension ref="A1:I217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
@@ -11128,8 +11128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0549D53A-9F65-1F4A-8A80-1A96C9AB66F8}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11796,6 +11796,9 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2014</v>
+      </c>
       <c r="B48" t="s">
         <v>54</v>
       </c>
@@ -11806,7 +11809,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2014</v>
+      </c>
       <c r="B49" t="s">
         <v>54</v>
       </c>
@@ -11817,7 +11823,10 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2014</v>
+      </c>
       <c r="B50" t="s">
         <v>54</v>
       </c>
@@ -11828,7 +11837,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2014</v>
+      </c>
       <c r="B51" t="s">
         <v>54</v>
       </c>
@@ -11839,7 +11851,10 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2014</v>
+      </c>
       <c r="B52" t="s">
         <v>54</v>
       </c>
@@ -11850,7 +11865,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2014</v>
+      </c>
       <c r="B53" t="s">
         <v>54</v>
       </c>
@@ -11861,7 +11879,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2014</v>
+      </c>
       <c r="B54" t="s">
         <v>56</v>
       </c>
@@ -11872,7 +11893,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2014</v>
+      </c>
       <c r="B55" t="s">
         <v>56</v>
       </c>
@@ -11883,7 +11907,10 @@
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2014</v>
+      </c>
       <c r="B56" t="s">
         <v>56</v>
       </c>
@@ -11894,7 +11921,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2014</v>
+      </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
@@ -11905,7 +11935,10 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2014</v>
+      </c>
       <c r="B58" t="s">
         <v>56</v>
       </c>
@@ -11916,7 +11949,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2014</v>
+      </c>
       <c r="B59" t="s">
         <v>56</v>
       </c>
@@ -11927,7 +11963,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2014</v>
+      </c>
       <c r="B60" t="s">
         <v>38</v>
       </c>
@@ -11938,7 +11977,10 @@
         <v>405</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2014</v>
+      </c>
       <c r="B61" t="s">
         <v>38</v>
       </c>
@@ -11949,7 +11991,10 @@
         <v>406</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2014</v>
+      </c>
       <c r="B62" t="s">
         <v>38</v>
       </c>
@@ -11960,7 +12005,10 @@
         <v>323</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2014</v>
+      </c>
       <c r="B63" t="s">
         <v>38</v>
       </c>
@@ -11971,7 +12019,10 @@
         <v>408</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2014</v>
+      </c>
       <c r="B64" t="s">
         <v>38</v>
       </c>
@@ -11982,7 +12033,10 @@
         <v>409</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2014</v>
+      </c>
       <c r="B65" t="s">
         <v>38</v>
       </c>
@@ -11993,7 +12047,10 @@
         <v>326</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2014</v>
+      </c>
       <c r="B66" t="s">
         <v>38</v>
       </c>
@@ -12004,7 +12061,10 @@
         <v>410</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2014</v>
+      </c>
       <c r="B67" t="s">
         <v>38</v>
       </c>
@@ -12015,7 +12075,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2014</v>
+      </c>
       <c r="B68" t="s">
         <v>38</v>
       </c>
@@ -12026,7 +12089,10 @@
         <v>412</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2014</v>
+      </c>
       <c r="B69" t="s">
         <v>38</v>
       </c>
@@ -12037,7 +12103,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2014</v>
+      </c>
       <c r="B70" t="s">
         <v>38</v>
       </c>
@@ -12048,7 +12117,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2014</v>
+      </c>
       <c r="B71" t="s">
         <v>38</v>
       </c>
@@ -12059,7 +12131,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>2014</v>
+      </c>
       <c r="B72" t="s">
         <v>38</v>
       </c>
@@ -12070,7 +12145,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2014</v>
+      </c>
       <c r="B73" t="s">
         <v>41</v>
       </c>
@@ -12081,7 +12159,10 @@
         <v>413</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>2014</v>
+      </c>
       <c r="B74" t="s">
         <v>41</v>
       </c>
@@ -12092,7 +12173,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2014</v>
+      </c>
       <c r="B75" t="s">
         <v>41</v>
       </c>
@@ -12103,7 +12187,10 @@
         <v>414</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2014</v>
+      </c>
       <c r="B76" t="s">
         <v>41</v>
       </c>
@@ -12114,7 +12201,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>2014</v>
+      </c>
       <c r="B77" t="s">
         <v>41</v>
       </c>
@@ -12125,7 +12215,10 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>2014</v>
+      </c>
       <c r="B78" t="s">
         <v>41</v>
       </c>
@@ -12136,7 +12229,10 @@
         <v>218</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2014</v>
+      </c>
       <c r="B79" t="s">
         <v>41</v>
       </c>
@@ -12147,7 +12243,10 @@
         <v>415</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2014</v>
+      </c>
       <c r="B80" t="s">
         <v>41</v>
       </c>
@@ -12158,7 +12257,10 @@
         <v>373</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>2014</v>
+      </c>
       <c r="B81" t="s">
         <v>41</v>
       </c>
@@ -12169,7 +12271,10 @@
         <v>221</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2014</v>
+      </c>
       <c r="B82" t="s">
         <v>41</v>
       </c>
@@ -12180,7 +12285,10 @@
         <v>417</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>2014</v>
+      </c>
       <c r="B83" t="s">
         <v>41</v>
       </c>
@@ -12191,7 +12299,10 @@
         <v>222</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>2014</v>
+      </c>
       <c r="B84" t="s">
         <v>41</v>
       </c>
@@ -12202,7 +12313,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>2014</v>
+      </c>
       <c r="B85" t="s">
         <v>41</v>
       </c>
@@ -12213,7 +12327,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>2014</v>
+      </c>
       <c r="B86" t="s">
         <v>41</v>
       </c>
@@ -12224,7 +12341,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>2014</v>
+      </c>
       <c r="B87" t="s">
         <v>41</v>
       </c>
@@ -12235,7 +12355,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>2014</v>
+      </c>
       <c r="B88" t="s">
         <v>44</v>
       </c>
@@ -12246,7 +12369,10 @@
         <v>418</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>2014</v>
+      </c>
       <c r="B89" t="s">
         <v>44</v>
       </c>
@@ -12257,7 +12383,10 @@
         <v>419</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>2014</v>
+      </c>
       <c r="B90" t="s">
         <v>44</v>
       </c>
@@ -12268,7 +12397,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>2014</v>
+      </c>
       <c r="B91" t="s">
         <v>44</v>
       </c>
@@ -12279,7 +12411,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>2014</v>
+      </c>
       <c r="B92" t="s">
         <v>44</v>
       </c>
@@ -12290,7 +12425,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>2014</v>
+      </c>
       <c r="B93" t="s">
         <v>44</v>
       </c>
@@ -12301,7 +12439,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>2014</v>
+      </c>
       <c r="B94" t="s">
         <v>47</v>
       </c>
@@ -12312,7 +12453,10 @@
         <v>421</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>2014</v>
+      </c>
       <c r="B95" t="s">
         <v>47</v>
       </c>
@@ -12323,7 +12467,10 @@
         <v>450</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>2014</v>
+      </c>
       <c r="B96" t="s">
         <v>47</v>
       </c>
@@ -12334,7 +12481,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>2014</v>
+      </c>
       <c r="B97" t="s">
         <v>47</v>
       </c>
@@ -12345,7 +12495,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>2014</v>
+      </c>
       <c r="B98" t="s">
         <v>47</v>
       </c>
@@ -12356,7 +12509,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>2014</v>
+      </c>
       <c r="B99" t="s">
         <v>47</v>
       </c>
@@ -12367,7 +12523,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>2014</v>
+      </c>
       <c r="B100" t="s">
         <v>67</v>
       </c>
@@ -12378,7 +12537,10 @@
         <v>424</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>2014</v>
+      </c>
       <c r="B101" t="s">
         <v>67</v>
       </c>
@@ -12389,7 +12551,10 @@
         <v>451</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>2014</v>
+      </c>
       <c r="B102" t="s">
         <v>67</v>
       </c>
@@ -12400,7 +12565,10 @@
         <v>227</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>2014</v>
+      </c>
       <c r="B103" t="s">
         <v>67</v>
       </c>
@@ -12411,7 +12579,10 @@
         <v>452</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>2014</v>
+      </c>
       <c r="B104" t="s">
         <v>67</v>
       </c>
@@ -12422,7 +12593,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>2014</v>
+      </c>
       <c r="B105" t="s">
         <v>67</v>
       </c>
@@ -12433,7 +12607,10 @@
         <v>229</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>2014</v>
+      </c>
       <c r="B106" t="s">
         <v>67</v>
       </c>
@@ -12444,7 +12621,10 @@
         <v>230</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>2014</v>
+      </c>
       <c r="B107" t="s">
         <v>67</v>
       </c>
@@ -12455,7 +12635,10 @@
         <v>341</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>2014</v>
+      </c>
       <c r="B108" t="s">
         <v>67</v>
       </c>
@@ -12466,7 +12649,10 @@
         <v>222</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>2014</v>
+      </c>
       <c r="B109" t="s">
         <v>67</v>
       </c>
@@ -12477,7 +12663,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>2014</v>
+      </c>
       <c r="B110" t="s">
         <v>67</v>
       </c>
@@ -12488,7 +12677,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>2014</v>
+      </c>
       <c r="B111" t="s">
         <v>67</v>
       </c>
@@ -12499,7 +12691,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>2014</v>
+      </c>
       <c r="B112" t="s">
         <v>67</v>
       </c>
@@ -12510,7 +12705,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>2014</v>
+      </c>
       <c r="B113" t="s">
         <v>454</v>
       </c>
@@ -12521,7 +12719,10 @@
         <v>453</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>2014</v>
+      </c>
       <c r="B114" t="s">
         <v>454</v>
       </c>
@@ -12532,7 +12733,10 @@
         <v>137</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>2014</v>
+      </c>
       <c r="B115" t="s">
         <v>454</v>
       </c>
@@ -12543,7 +12747,10 @@
         <v>138</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>2014</v>
+      </c>
       <c r="B116" t="s">
         <v>454</v>
       </c>
@@ -12554,7 +12761,10 @@
         <v>139</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>2014</v>
+      </c>
       <c r="B117" t="s">
         <v>454</v>
       </c>
@@ -12565,7 +12775,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>2014</v>
+      </c>
       <c r="B118" t="s">
         <v>454</v>
       </c>
@@ -12576,7 +12789,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>2014</v>
+      </c>
       <c r="B119" t="s">
         <v>454</v>
       </c>
@@ -12587,7 +12803,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>2014</v>
+      </c>
       <c r="B120" t="s">
         <v>454</v>
       </c>
@@ -23300,7 +23519,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9942FE2-02FE-0447-8EFB-7DD7FBDD6A84}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:A108"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -23897,6 +24118,9 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2006</v>
+      </c>
       <c r="B43" t="s">
         <v>54</v>
       </c>
@@ -23908,6 +24132,9 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2006</v>
+      </c>
       <c r="B44" t="s">
         <v>54</v>
       </c>
@@ -23919,6 +24146,9 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2006</v>
+      </c>
       <c r="B45" t="s">
         <v>54</v>
       </c>
@@ -23930,6 +24160,9 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2006</v>
+      </c>
       <c r="B46" t="s">
         <v>54</v>
       </c>
@@ -23941,6 +24174,9 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2006</v>
+      </c>
       <c r="B47" t="s">
         <v>54</v>
       </c>
@@ -23952,6 +24188,9 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2006</v>
+      </c>
       <c r="B48" t="s">
         <v>56</v>
       </c>
@@ -23962,7 +24201,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2006</v>
+      </c>
       <c r="B49" t="s">
         <v>56</v>
       </c>
@@ -23973,7 +24215,10 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2006</v>
+      </c>
       <c r="B50" t="s">
         <v>56</v>
       </c>
@@ -23984,7 +24229,10 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2006</v>
+      </c>
       <c r="B51" t="s">
         <v>56</v>
       </c>
@@ -23995,7 +24243,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2006</v>
+      </c>
       <c r="B52" t="s">
         <v>56</v>
       </c>
@@ -24006,7 +24257,10 @@
         <v>360</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2006</v>
+      </c>
       <c r="B53" t="s">
         <v>38</v>
       </c>
@@ -24017,7 +24271,10 @@
         <v>321</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2006</v>
+      </c>
       <c r="B54" t="s">
         <v>38</v>
       </c>
@@ -24028,7 +24285,10 @@
         <v>322</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2006</v>
+      </c>
       <c r="B55" t="s">
         <v>38</v>
       </c>
@@ -24039,7 +24299,10 @@
         <v>323</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2006</v>
+      </c>
       <c r="B56" t="s">
         <v>38</v>
       </c>
@@ -24050,7 +24313,10 @@
         <v>324</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2006</v>
+      </c>
       <c r="B57" t="s">
         <v>38</v>
       </c>
@@ -24061,7 +24327,10 @@
         <v>325</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2006</v>
+      </c>
       <c r="B58" t="s">
         <v>38</v>
       </c>
@@ -24072,7 +24341,10 @@
         <v>326</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2006</v>
+      </c>
       <c r="B59" t="s">
         <v>38</v>
       </c>
@@ -24083,7 +24355,10 @@
         <v>327</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2006</v>
+      </c>
       <c r="B60" t="s">
         <v>38</v>
       </c>
@@ -24094,7 +24369,10 @@
         <v>328</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2006</v>
+      </c>
       <c r="B61" t="s">
         <v>38</v>
       </c>
@@ -24105,7 +24383,10 @@
         <v>329</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2006</v>
+      </c>
       <c r="B62" t="s">
         <v>38</v>
       </c>
@@ -24116,7 +24397,10 @@
         <v>238</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2006</v>
+      </c>
       <c r="B63" t="s">
         <v>38</v>
       </c>
@@ -24127,7 +24411,10 @@
         <v>225</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2006</v>
+      </c>
       <c r="B64" t="s">
         <v>38</v>
       </c>
@@ -24138,7 +24425,10 @@
         <v>361</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2006</v>
+      </c>
       <c r="B65" t="s">
         <v>41</v>
       </c>
@@ -24149,7 +24439,10 @@
         <v>330</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2006</v>
+      </c>
       <c r="B66" t="s">
         <v>41</v>
       </c>
@@ -24160,7 +24453,10 @@
         <v>264</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2006</v>
+      </c>
       <c r="B67" t="s">
         <v>41</v>
       </c>
@@ -24171,7 +24467,10 @@
         <v>217</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2006</v>
+      </c>
       <c r="B68" t="s">
         <v>41</v>
       </c>
@@ -24182,7 +24481,10 @@
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2006</v>
+      </c>
       <c r="B69" t="s">
         <v>41</v>
       </c>
@@ -24193,7 +24495,10 @@
         <v>265</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2006</v>
+      </c>
       <c r="B70" t="s">
         <v>41</v>
       </c>
@@ -24204,7 +24509,10 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2006</v>
+      </c>
       <c r="B71" t="s">
         <v>41</v>
       </c>
@@ -24215,7 +24523,10 @@
         <v>332</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>2006</v>
+      </c>
       <c r="B72" t="s">
         <v>41</v>
       </c>
@@ -24226,7 +24537,10 @@
         <v>333</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2006</v>
+      </c>
       <c r="B73" t="s">
         <v>41</v>
       </c>
@@ -24237,7 +24551,10 @@
         <v>267</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>2006</v>
+      </c>
       <c r="B74" t="s">
         <v>41</v>
       </c>
@@ -24248,7 +24565,10 @@
         <v>334</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2006</v>
+      </c>
       <c r="B75" t="s">
         <v>41</v>
       </c>
@@ -24259,7 +24579,10 @@
         <v>272</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2006</v>
+      </c>
       <c r="B76" t="s">
         <v>41</v>
       </c>
@@ -24270,7 +24593,10 @@
         <v>238</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>2006</v>
+      </c>
       <c r="B77" t="s">
         <v>41</v>
       </c>
@@ -24281,7 +24607,10 @@
         <v>225</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>2006</v>
+      </c>
       <c r="B78" t="s">
         <v>41</v>
       </c>
@@ -24292,7 +24621,10 @@
         <v>361</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2006</v>
+      </c>
       <c r="B79" t="s">
         <v>44</v>
       </c>
@@ -24303,7 +24635,10 @@
         <v>335</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2006</v>
+      </c>
       <c r="B80" t="s">
         <v>44</v>
       </c>
@@ -24314,7 +24649,10 @@
         <v>336</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>2006</v>
+      </c>
       <c r="B81" t="s">
         <v>44</v>
       </c>
@@ -24325,7 +24663,10 @@
         <v>238</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2006</v>
+      </c>
       <c r="B82" t="s">
         <v>44</v>
       </c>
@@ -24336,7 +24677,10 @@
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>2006</v>
+      </c>
       <c r="B83" t="s">
         <v>44</v>
       </c>
@@ -24347,7 +24691,10 @@
         <v>361</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>2006</v>
+      </c>
       <c r="B84" t="s">
         <v>47</v>
       </c>
@@ -24358,7 +24705,10 @@
         <v>337</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>2006</v>
+      </c>
       <c r="B85" t="s">
         <v>47</v>
       </c>
@@ -24369,7 +24719,10 @@
         <v>338</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>2006</v>
+      </c>
       <c r="B86" t="s">
         <v>47</v>
       </c>
@@ -24380,7 +24733,10 @@
         <v>238</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>2006</v>
+      </c>
       <c r="B87" t="s">
         <v>47</v>
       </c>
@@ -24391,7 +24747,10 @@
         <v>225</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>2006</v>
+      </c>
       <c r="B88" t="s">
         <v>47</v>
       </c>
@@ -24402,7 +24761,10 @@
         <v>361</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>2006</v>
+      </c>
       <c r="B89" t="s">
         <v>67</v>
       </c>
@@ -24413,7 +24775,10 @@
         <v>365</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>2006</v>
+      </c>
       <c r="B90" t="s">
         <v>67</v>
       </c>
@@ -24424,7 +24789,10 @@
         <v>366</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>2006</v>
+      </c>
       <c r="B91" t="s">
         <v>67</v>
       </c>
@@ -24435,7 +24803,10 @@
         <v>271</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>2006</v>
+      </c>
       <c r="B92" t="s">
         <v>67</v>
       </c>
@@ -24446,7 +24817,10 @@
         <v>228</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>2006</v>
+      </c>
       <c r="B93" t="s">
         <v>67</v>
       </c>
@@ -24457,7 +24831,10 @@
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>2006</v>
+      </c>
       <c r="B94" t="s">
         <v>67</v>
       </c>
@@ -24468,7 +24845,10 @@
         <v>230</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>2006</v>
+      </c>
       <c r="B95" t="s">
         <v>67</v>
       </c>
@@ -24479,7 +24859,10 @@
         <v>341</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>2006</v>
+      </c>
       <c r="B96" t="s">
         <v>67</v>
       </c>
@@ -24490,7 +24873,10 @@
         <v>272</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>2006</v>
+      </c>
       <c r="B97" t="s">
         <v>67</v>
       </c>
@@ -24501,7 +24887,10 @@
         <v>238</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>2006</v>
+      </c>
       <c r="B98" t="s">
         <v>67</v>
       </c>
@@ -24512,7 +24901,10 @@
         <v>225</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>2006</v>
+      </c>
       <c r="B99" t="s">
         <v>67</v>
       </c>
@@ -24523,7 +24915,10 @@
         <v>361</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>2006</v>
+      </c>
       <c r="B100" t="s">
         <v>70</v>
       </c>
@@ -24534,7 +24929,10 @@
         <v>232</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>2006</v>
+      </c>
       <c r="B101" t="s">
         <v>70</v>
       </c>
@@ -24545,7 +24943,10 @@
         <v>233</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>2006</v>
+      </c>
       <c r="B102" t="s">
         <v>70</v>
       </c>
@@ -24556,7 +24957,10 @@
         <v>234</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>2006</v>
+      </c>
       <c r="B103" t="s">
         <v>70</v>
       </c>
@@ -24567,7 +24971,10 @@
         <v>235</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>2006</v>
+      </c>
       <c r="B104" t="s">
         <v>70</v>
       </c>
@@ -24578,7 +24985,10 @@
         <v>236</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>2006</v>
+      </c>
       <c r="B105" t="s">
         <v>70</v>
       </c>
@@ -24589,7 +24999,10 @@
         <v>237</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>2006</v>
+      </c>
       <c r="B106" t="s">
         <v>70</v>
       </c>
@@ -24600,7 +25013,10 @@
         <v>238</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>2006</v>
+      </c>
       <c r="B107" t="s">
         <v>70</v>
       </c>
@@ -24611,7 +25027,10 @@
         <v>225</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>2006</v>
+      </c>
       <c r="B108" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Fix two voting columns coded as "Non-Hipsanic" in 1994
</commit_message>
<xml_diff>
--- a/data-raw/catalog.xlsx
+++ b/data-raw/catalog.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaylee/Desktop/cpsvote/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB83E937-03BF-734D-9FD5-B38971454BBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7A2B8A-227D-C144-8645-35F7597F2EDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="1bbBXZEuvpXUWOM4H2dfSf4qEe/w9aOR03O17HJVfeBciv1kJfxQcX2uJxQ8G/6hB+8cpQEqFL6wwb4yaAP/1w==" workbookSaltValue="po6nkgUJ66gqb2vNNVbSbw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="4840" windowWidth="27640" windowHeight="16940" activeTab="11" xr2:uid="{F3FFB08B-FE6D-ED48-9525-18B361D5DDB4}"/>
+    <workbookView xWindow="1500" yWindow="4840" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{F3FFB08B-FE6D-ED48-9525-18B361D5DDB4}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -11128,7 +11128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0549D53A-9F65-1F4A-8A80-1A96C9AB66F8}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="A47" sqref="A47:A120"/>
     </sheetView>
   </sheetViews>
@@ -16221,7 +16221,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C16B797-997F-2E4F-8A09-DA0915397AE8}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -16614,7 +16616,7 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -16670,7 +16672,7 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Okay one last smart quote fix
</commit_message>
<xml_diff>
--- a/data-raw/catalog.xlsx
+++ b/data-raw/catalog.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaylee/Desktop/cpsvote/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD743F1-0D46-DE42-B790-F437A4C93F09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7806D219-CCFD-B047-BBEB-D27BF53F16BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="1bbBXZEuvpXUWOM4H2dfSf4qEe/w9aOR03O17HJVfeBciv1kJfxQcX2uJxQ8G/6hB+8cpQEqFL6wwb4yaAP/1w==" workbookSaltValue="po6nkgUJ66gqb2vNNVbSbw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{F3FFB08B-FE6D-ED48-9525-18B361D5DDB4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{F3FFB08B-FE6D-ED48-9525-18B361D5DDB4}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4422" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4422" uniqueCount="470">
   <si>
     <t>year</t>
   </si>
@@ -1033,18 +1033,6 @@
     <t xml:space="preserve">Other reason </t>
   </si>
   <si>
-    <t xml:space="preserve">Illness or disability (own or family’s) </t>
-  </si>
-  <si>
-    <t>Not interested, felt my vote wouldn’t make a difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Didn’t like candidates or campaign issues </t>
-  </si>
-  <si>
-    <t>Registration problems (i.e. didn’t receive absentee ballot, not registered in current location)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Inconvenient hours, polling place or hours or lines too long </t>
   </si>
   <si>
@@ -1133,9 +1121,6 @@
   </si>
   <si>
     <t xml:space="preserve">EDITED UNIVERSE: PES6 = 1,2,-2,-3,-9; PES4 = 1-11, -2,-3,-9 </t>
-  </si>
-  <si>
-    <t>At a department of motor vehicles (for example, when obtaining a driver’s license or other identification card)</t>
   </si>
   <si>
     <t xml:space="preserve">At a public assistance agency (for example, a Medicaid, AFDC, or Food Stamps office, an office serving disabled persons, or an unemployment office) </t>
@@ -1831,7 +1816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFB3A44-3E53-2642-A3DE-5CB8717D98DA}">
   <dimension ref="A1:I217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
@@ -1847,7 +1832,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2134,7 +2119,7 @@
         <v>41</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E11" s="3">
         <v>819</v>
@@ -2163,7 +2148,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E12" s="3">
         <v>821</v>
@@ -2279,7 +2264,7 @@
         <v>51</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E16" s="3">
         <v>101</v>
@@ -2499,7 +2484,7 @@
         <v>56</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E24" s="3">
         <v>817</v>
@@ -2528,7 +2513,7 @@
         <v>38</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E25" s="3">
         <v>819</v>
@@ -2557,7 +2542,7 @@
         <v>41</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="E26" s="3">
         <v>821</v>
@@ -2586,7 +2571,7 @@
         <v>44</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="E27" s="3">
         <v>823</v>
@@ -2615,7 +2600,7 @@
         <v>47</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="E28" s="3">
         <v>825</v>
@@ -2644,7 +2629,7 @@
         <v>67</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E29" s="3">
         <v>827</v>
@@ -2757,7 +2742,7 @@
         <v>51</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E33" s="3">
         <v>101</v>
@@ -2977,7 +2962,7 @@
         <v>56</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E41" s="3">
         <v>859</v>
@@ -3006,7 +2991,7 @@
         <v>38</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E42" s="3">
         <v>861</v>
@@ -3035,7 +3020,7 @@
         <v>41</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="E43" s="3">
         <v>863</v>
@@ -3064,7 +3049,7 @@
         <v>44</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="E44" s="3">
         <v>865</v>
@@ -3093,7 +3078,7 @@
         <v>47</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="E45" s="3">
         <v>867</v>
@@ -3122,7 +3107,7 @@
         <v>67</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E46" s="3">
         <v>869</v>
@@ -3235,7 +3220,7 @@
         <v>51</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E50" s="3">
         <v>101</v>
@@ -3455,7 +3440,7 @@
         <v>56</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E58" s="3">
         <v>859</v>
@@ -3484,7 +3469,7 @@
         <v>38</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E59" s="3">
         <v>861</v>
@@ -3513,7 +3498,7 @@
         <v>41</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="E60" s="3">
         <v>863</v>
@@ -3542,7 +3527,7 @@
         <v>44</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="E61" s="3">
         <v>865</v>
@@ -3571,7 +3556,7 @@
         <v>47</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="E62" s="3">
         <v>867</v>
@@ -3600,7 +3585,7 @@
         <v>67</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E63" s="3">
         <v>869</v>
@@ -3713,7 +3698,7 @@
         <v>51</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E67" s="3">
         <v>101</v>
@@ -3933,7 +3918,7 @@
         <v>56</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E75" s="3">
         <v>859</v>
@@ -3962,7 +3947,7 @@
         <v>38</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E76" s="3">
         <v>861</v>
@@ -3991,7 +3976,7 @@
         <v>41</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="E77" s="3">
         <v>863</v>
@@ -4020,7 +4005,7 @@
         <v>44</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="E78" s="3">
         <v>865</v>
@@ -4049,7 +4034,7 @@
         <v>47</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="E79" s="3">
         <v>867</v>
@@ -4078,7 +4063,7 @@
         <v>67</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E80" s="3">
         <v>869</v>
@@ -4191,7 +4176,7 @@
         <v>76</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E84" s="3">
         <v>101</v>
@@ -4414,7 +4399,7 @@
         <v>56</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E92" s="3">
         <v>879</v>
@@ -4443,7 +4428,7 @@
         <v>38</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E93" s="3">
         <v>881</v>
@@ -4472,7 +4457,7 @@
         <v>41</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E94" s="3">
         <v>883</v>
@@ -4501,7 +4486,7 @@
         <v>44</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E95" s="3">
         <v>885</v>
@@ -4530,7 +4515,7 @@
         <v>47</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E96" s="3">
         <v>887</v>
@@ -4559,7 +4544,7 @@
         <v>67</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E97" s="3">
         <v>889</v>
@@ -4574,7 +4559,7 @@
         <v>91</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -4672,7 +4657,7 @@
         <v>76</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E101" s="3">
         <v>101</v>
@@ -4892,7 +4877,7 @@
         <v>56</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E109" s="3">
         <v>953</v>
@@ -4921,7 +4906,7 @@
         <v>38</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E110" s="3">
         <v>955</v>
@@ -4950,7 +4935,7 @@
         <v>41</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E111" s="3">
         <v>957</v>
@@ -4979,7 +4964,7 @@
         <v>44</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E112" s="3">
         <v>959</v>
@@ -5008,7 +4993,7 @@
         <v>47</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E113" s="3">
         <v>961</v>
@@ -5020,7 +5005,7 @@
         <v>15</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I113" s="3" t="s">
         <v>90</v>
@@ -5037,7 +5022,7 @@
         <v>67</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E114" s="3">
         <v>963</v>
@@ -5049,10 +5034,10 @@
         <v>15</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
@@ -5078,7 +5063,7 @@
         <v>15</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I115" s="3" t="s">
         <v>27</v>
@@ -5150,7 +5135,7 @@
         <v>76</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E118" s="3">
         <v>101</v>
@@ -5356,7 +5341,7 @@
         <v>15</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -5370,7 +5355,7 @@
         <v>56</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E126" s="3">
         <v>953</v>
@@ -5382,7 +5367,7 @@
         <v>15</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="I126" s="3" t="s">
         <v>95</v>
@@ -5399,7 +5384,7 @@
         <v>38</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E127" s="3">
         <v>955</v>
@@ -5411,7 +5396,7 @@
         <v>15</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="I127" s="3" t="s">
         <v>96</v>
@@ -5428,7 +5413,7 @@
         <v>41</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E128" s="3">
         <v>957</v>
@@ -5440,10 +5425,10 @@
         <v>15</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -5457,7 +5442,7 @@
         <v>44</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E129" s="3">
         <v>959</v>
@@ -5469,7 +5454,7 @@
         <v>15</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="I129" s="3" t="s">
         <v>88</v>
@@ -5486,7 +5471,7 @@
         <v>47</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E130" s="3">
         <v>961</v>
@@ -5498,7 +5483,7 @@
         <v>15</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="I130" s="3" t="s">
         <v>90</v>
@@ -5515,7 +5500,7 @@
         <v>67</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E131" s="3">
         <v>963</v>
@@ -5527,10 +5512,10 @@
         <v>15</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
@@ -5556,7 +5541,7 @@
         <v>15</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I132" s="3" t="s">
         <v>27</v>
@@ -5628,7 +5613,7 @@
         <v>76</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E135" s="3">
         <v>101</v>
@@ -5834,7 +5819,7 @@
         <v>15</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -5848,7 +5833,7 @@
         <v>56</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E143" s="3">
         <v>953</v>
@@ -5860,7 +5845,7 @@
         <v>15</v>
       </c>
       <c r="H143" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="I143" s="3" t="s">
         <v>95</v>
@@ -5877,7 +5862,7 @@
         <v>38</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E144" s="3">
         <v>955</v>
@@ -5889,7 +5874,7 @@
         <v>15</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="I144" s="3" t="s">
         <v>96</v>
@@ -5906,7 +5891,7 @@
         <v>41</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E145" s="3">
         <v>957</v>
@@ -5918,10 +5903,10 @@
         <v>15</v>
       </c>
       <c r="H145" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="I145" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -5935,7 +5920,7 @@
         <v>44</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E146" s="3">
         <v>959</v>
@@ -5947,7 +5932,7 @@
         <v>15</v>
       </c>
       <c r="H146" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="I146" s="3" t="s">
         <v>88</v>
@@ -5964,7 +5949,7 @@
         <v>47</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E147" s="3">
         <v>961</v>
@@ -5976,10 +5961,10 @@
         <v>15</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="I147" s="3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -5993,7 +5978,7 @@
         <v>67</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E148" s="3">
         <v>963</v>
@@ -6005,10 +5990,10 @@
         <v>15</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -6034,7 +6019,7 @@
         <v>15</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I149" s="3" t="s">
         <v>27</v>
@@ -6106,7 +6091,7 @@
         <v>76</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E152" s="3">
         <v>101</v>
@@ -6132,7 +6117,7 @@
         <v>2012</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>18</v>
@@ -6147,7 +6132,7 @@
         <v>10</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I153" s="3" t="s">
         <v>92</v>
@@ -6312,7 +6297,7 @@
         <v>15</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -6326,7 +6311,7 @@
         <v>56</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E160" s="3">
         <v>953</v>
@@ -6338,7 +6323,7 @@
         <v>15</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I160" s="3" t="s">
         <v>58</v>
@@ -6355,7 +6340,7 @@
         <v>38</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E161" s="3">
         <v>955</v>
@@ -6367,7 +6352,7 @@
         <v>15</v>
       </c>
       <c r="H161" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="I161" s="3" t="s">
         <v>96</v>
@@ -6384,7 +6369,7 @@
         <v>41</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E162" s="3">
         <v>957</v>
@@ -6396,7 +6381,7 @@
         <v>15</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="I162" s="3" t="s">
         <v>86</v>
@@ -6413,7 +6398,7 @@
         <v>44</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E163" s="3">
         <v>959</v>
@@ -6425,7 +6410,7 @@
         <v>15</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="I163" s="3" t="s">
         <v>88</v>
@@ -6442,7 +6427,7 @@
         <v>47</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E164" s="3">
         <v>961</v>
@@ -6454,10 +6439,10 @@
         <v>15</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="I164" s="3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
@@ -6471,7 +6456,7 @@
         <v>67</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E165" s="3">
         <v>963</v>
@@ -6483,10 +6468,10 @@
         <v>15</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="I165" s="3" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
@@ -6512,7 +6497,7 @@
         <v>15</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I166" s="3" t="s">
         <v>27</v>
@@ -6584,7 +6569,7 @@
         <v>76</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E169" s="3">
         <v>101</v>
@@ -6610,7 +6595,7 @@
         <v>2014</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>18</v>
@@ -6625,7 +6610,7 @@
         <v>10</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I170" s="3" t="s">
         <v>92</v>
@@ -6790,7 +6775,7 @@
         <v>15</v>
       </c>
       <c r="H176" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
@@ -6804,7 +6789,7 @@
         <v>56</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E177" s="3">
         <v>953</v>
@@ -6816,7 +6801,7 @@
         <v>15</v>
       </c>
       <c r="H177" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="I177" s="3" t="s">
         <v>58</v>
@@ -6833,7 +6818,7 @@
         <v>38</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E178" s="3">
         <v>955</v>
@@ -6845,7 +6830,7 @@
         <v>15</v>
       </c>
       <c r="H178" s="3" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I178" s="3" t="s">
         <v>85</v>
@@ -6862,7 +6847,7 @@
         <v>41</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E179" s="3">
         <v>957</v>
@@ -6891,7 +6876,7 @@
         <v>44</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E180" s="3">
         <v>959</v>
@@ -6920,7 +6905,7 @@
         <v>47</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E181" s="3">
         <v>961</v>
@@ -6932,10 +6917,10 @@
         <v>15</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="I181" s="3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
@@ -6949,7 +6934,7 @@
         <v>67</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E182" s="3">
         <v>963</v>
@@ -6961,7 +6946,7 @@
         <v>15</v>
       </c>
       <c r="H182" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I182" s="3" t="s">
         <v>64</v>
@@ -6975,7 +6960,7 @@
         <v>2014</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>48</v>
@@ -6993,7 +6978,7 @@
         <v>49</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
@@ -7062,7 +7047,7 @@
         <v>76</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E186" s="3">
         <v>101</v>
@@ -7088,7 +7073,7 @@
         <v>2016</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>18</v>
@@ -7103,7 +7088,7 @@
         <v>10</v>
       </c>
       <c r="H187" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I187" s="3" t="s">
         <v>92</v>
@@ -7268,7 +7253,7 @@
         <v>15</v>
       </c>
       <c r="H193" s="3" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.2">
@@ -7282,7 +7267,7 @@
         <v>56</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E194" s="3">
         <v>953</v>
@@ -7294,7 +7279,7 @@
         <v>15</v>
       </c>
       <c r="H194" s="3" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="I194" s="3" t="s">
         <v>95</v>
@@ -7311,7 +7296,7 @@
         <v>38</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E195" s="3">
         <v>955</v>
@@ -7323,7 +7308,7 @@
         <v>15</v>
       </c>
       <c r="H195" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="I195" s="3" t="s">
         <v>85</v>
@@ -7340,7 +7325,7 @@
         <v>41</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E196" s="3">
         <v>957</v>
@@ -7352,10 +7337,10 @@
         <v>15</v>
       </c>
       <c r="H196" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="I196" s="3" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
@@ -7369,7 +7354,7 @@
         <v>44</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E197" s="3">
         <v>959</v>
@@ -7381,7 +7366,7 @@
         <v>15</v>
       </c>
       <c r="H197" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="I197" s="3" t="s">
         <v>62</v>
@@ -7398,7 +7383,7 @@
         <v>47</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E198" s="3">
         <v>961</v>
@@ -7410,10 +7395,10 @@
         <v>15</v>
       </c>
       <c r="H198" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="I198" s="3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.2">
@@ -7427,7 +7412,7 @@
         <v>67</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E199" s="3">
         <v>963</v>
@@ -7439,10 +7424,10 @@
         <v>15</v>
       </c>
       <c r="H199" s="3" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="I199" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.2">
@@ -7453,7 +7438,7 @@
         <v>2016</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>48</v>
@@ -7468,7 +7453,7 @@
         <v>15</v>
       </c>
       <c r="H200" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I200" s="3" t="s">
         <v>27</v>
@@ -7540,7 +7525,7 @@
         <v>76</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E203" s="3">
         <v>101</v>
@@ -7566,7 +7551,7 @@
         <v>2018</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D204" s="3" t="s">
         <v>18</v>
@@ -7581,7 +7566,7 @@
         <v>10</v>
       </c>
       <c r="H204" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I204" s="3" t="s">
         <v>92</v>
@@ -7746,7 +7731,7 @@
         <v>15</v>
       </c>
       <c r="H210" s="3" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.2">
@@ -7760,7 +7745,7 @@
         <v>56</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E211" s="3">
         <v>1003</v>
@@ -7772,7 +7757,7 @@
         <v>15</v>
       </c>
       <c r="H211" s="3" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="I211" s="3" t="s">
         <v>95</v>
@@ -7789,7 +7774,7 @@
         <v>38</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E212" s="3">
         <v>1005</v>
@@ -7801,7 +7786,7 @@
         <v>15</v>
       </c>
       <c r="H212" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="I212" s="3" t="s">
         <v>85</v>
@@ -7818,7 +7803,7 @@
         <v>41</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E213" s="3">
         <v>1007</v>
@@ -7830,10 +7815,10 @@
         <v>15</v>
       </c>
       <c r="H213" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="I213" s="3" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.2">
@@ -7847,7 +7832,7 @@
         <v>44</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E214" s="3">
         <v>1009</v>
@@ -7859,7 +7844,7 @@
         <v>15</v>
       </c>
       <c r="H214" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="I214" s="3" t="s">
         <v>62</v>
@@ -7876,7 +7861,7 @@
         <v>47</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E215" s="3">
         <v>1011</v>
@@ -7888,10 +7873,10 @@
         <v>15</v>
       </c>
       <c r="H215" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="I215" s="3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.2">
@@ -7905,7 +7890,7 @@
         <v>67</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="E216" s="3">
         <v>1013</v>
@@ -7917,10 +7902,10 @@
         <v>15</v>
       </c>
       <c r="H216" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.2">
@@ -7946,7 +7931,7 @@
         <v>15</v>
       </c>
       <c r="H217" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I217" s="3" t="s">
         <v>27</v>
@@ -8977,7 +8962,7 @@
         <v>179</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -9005,7 +8990,7 @@
         <v>283</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -9075,7 +9060,7 @@
         <v>167</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -9089,7 +9074,7 @@
         <v>168</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -9145,7 +9130,7 @@
         <v>167</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -9159,7 +9144,7 @@
         <v>168</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -9215,7 +9200,7 @@
         <v>167</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -9229,7 +9214,7 @@
         <v>168</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -9257,7 +9242,7 @@
         <v>175</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -9313,7 +9298,7 @@
         <v>179</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -9681,7 +9666,7 @@
         <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -9709,7 +9694,7 @@
         <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -9751,7 +9736,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -9765,7 +9750,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -9905,7 +9890,7 @@
         <v>282</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -9975,7 +9960,7 @@
         <v>287</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -10031,7 +10016,7 @@
         <v>291</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -10059,7 +10044,7 @@
         <v>293</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -10084,10 +10069,10 @@
         <v>79</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -10098,7 +10083,7 @@
         <v>79</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>314</v>
@@ -10112,10 +10097,10 @@
         <v>79</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -10126,10 +10111,10 @@
         <v>79</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -10140,10 +10125,10 @@
         <v>79</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -10325,7 +10310,7 @@
         <v>167</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -10339,7 +10324,7 @@
         <v>168</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -10353,7 +10338,7 @@
         <v>174</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -10367,7 +10352,7 @@
         <v>175</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -10381,7 +10366,7 @@
         <v>176</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -10409,7 +10394,7 @@
         <v>178</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -10423,7 +10408,7 @@
         <v>179</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -10437,7 +10422,7 @@
         <v>180</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -10493,7 +10478,7 @@
         <v>167</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -10521,7 +10506,7 @@
         <v>174</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -10577,7 +10562,7 @@
         <v>178</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -10591,7 +10576,7 @@
         <v>179</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -10619,7 +10604,7 @@
         <v>283</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -10689,7 +10674,7 @@
         <v>167</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -10703,7 +10688,7 @@
         <v>168</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -10759,7 +10744,7 @@
         <v>167</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -10773,7 +10758,7 @@
         <v>168</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -10829,7 +10814,7 @@
         <v>167</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -10843,7 +10828,7 @@
         <v>168</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -10871,7 +10856,7 @@
         <v>175</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -10913,7 +10898,7 @@
         <v>178</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -10927,7 +10912,7 @@
         <v>179</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -11184,7 +11169,7 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -11198,7 +11183,7 @@
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -11212,7 +11197,7 @@
         <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -11226,7 +11211,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -11240,7 +11225,7 @@
         <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -11254,7 +11239,7 @@
         <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -11268,7 +11253,7 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -11282,7 +11267,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -11310,7 +11295,7 @@
         <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -11422,7 +11407,7 @@
         <v>141</v>
       </c>
       <c r="D21" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -11436,7 +11421,7 @@
         <v>163</v>
       </c>
       <c r="D22" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -11450,7 +11435,7 @@
         <v>164</v>
       </c>
       <c r="D23" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -11464,7 +11449,7 @@
         <v>165</v>
       </c>
       <c r="D24" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -11478,7 +11463,7 @@
         <v>279</v>
       </c>
       <c r="D25" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -11492,7 +11477,7 @@
         <v>280</v>
       </c>
       <c r="D26" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -11506,7 +11491,7 @@
         <v>281</v>
       </c>
       <c r="D27" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -11520,7 +11505,7 @@
         <v>282</v>
       </c>
       <c r="D28" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -11534,7 +11519,7 @@
         <v>283</v>
       </c>
       <c r="D29" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -11548,7 +11533,7 @@
         <v>284</v>
       </c>
       <c r="D30" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -11562,7 +11547,7 @@
         <v>285</v>
       </c>
       <c r="D31" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -11576,7 +11561,7 @@
         <v>286</v>
       </c>
       <c r="D32" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -11590,7 +11575,7 @@
         <v>287</v>
       </c>
       <c r="D33" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -11604,7 +11589,7 @@
         <v>288</v>
       </c>
       <c r="D34" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -11618,7 +11603,7 @@
         <v>289</v>
       </c>
       <c r="D35" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -11632,7 +11617,7 @@
         <v>290</v>
       </c>
       <c r="D36" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -11646,7 +11631,7 @@
         <v>291</v>
       </c>
       <c r="D37" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -11660,7 +11645,7 @@
         <v>292</v>
       </c>
       <c r="D38" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -11674,7 +11659,7 @@
         <v>293</v>
       </c>
       <c r="D39" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -11688,7 +11673,7 @@
         <v>294</v>
       </c>
       <c r="D40" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -11699,10 +11684,10 @@
         <v>79</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D41" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -11713,10 +11698,10 @@
         <v>79</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D42" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -11727,10 +11712,10 @@
         <v>79</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D43" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -11741,10 +11726,10 @@
         <v>79</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D44" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -11755,10 +11740,10 @@
         <v>79</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D45" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -11786,7 +11771,7 @@
         <v>168</v>
       </c>
       <c r="D47" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -11828,7 +11813,7 @@
         <v>181</v>
       </c>
       <c r="D50" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -11912,7 +11897,7 @@
         <v>181</v>
       </c>
       <c r="D56" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -11968,7 +11953,7 @@
         <v>167</v>
       </c>
       <c r="D60" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -11982,7 +11967,7 @@
         <v>168</v>
       </c>
       <c r="D61" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -12010,7 +11995,7 @@
         <v>175</v>
       </c>
       <c r="D63" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -12024,7 +12009,7 @@
         <v>176</v>
       </c>
       <c r="D64" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -12052,7 +12037,7 @@
         <v>178</v>
       </c>
       <c r="D66" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -12066,7 +12051,7 @@
         <v>179</v>
       </c>
       <c r="D67" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -12080,7 +12065,7 @@
         <v>180</v>
       </c>
       <c r="D68" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -12094,7 +12079,7 @@
         <v>181</v>
       </c>
       <c r="D69" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -12150,7 +12135,7 @@
         <v>167</v>
       </c>
       <c r="D73" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -12178,7 +12163,7 @@
         <v>174</v>
       </c>
       <c r="D75" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -12234,7 +12219,7 @@
         <v>178</v>
       </c>
       <c r="D79" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -12248,7 +12233,7 @@
         <v>179</v>
       </c>
       <c r="D80" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -12276,7 +12261,7 @@
         <v>283</v>
       </c>
       <c r="D82" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -12304,7 +12289,7 @@
         <v>181</v>
       </c>
       <c r="D84" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -12360,7 +12345,7 @@
         <v>167</v>
       </c>
       <c r="D88" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -12374,7 +12359,7 @@
         <v>168</v>
       </c>
       <c r="D89" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -12388,7 +12373,7 @@
         <v>181</v>
       </c>
       <c r="D90" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -12444,7 +12429,7 @@
         <v>167</v>
       </c>
       <c r="D94" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -12458,7 +12443,7 @@
         <v>168</v>
       </c>
       <c r="D95" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -12472,7 +12457,7 @@
         <v>181</v>
       </c>
       <c r="D96" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -12528,7 +12513,7 @@
         <v>167</v>
       </c>
       <c r="D100" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -12542,7 +12527,7 @@
         <v>168</v>
       </c>
       <c r="D101" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -12570,7 +12555,7 @@
         <v>175</v>
       </c>
       <c r="D103" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -12626,7 +12611,7 @@
         <v>179</v>
       </c>
       <c r="D107" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -12654,7 +12639,7 @@
         <v>181</v>
       </c>
       <c r="D109" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -12704,13 +12689,13 @@
         <v>2014</v>
       </c>
       <c r="B113" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>167</v>
       </c>
       <c r="D113" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -12718,7 +12703,7 @@
         <v>2014</v>
       </c>
       <c r="B114" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>168</v>
@@ -12732,7 +12717,7 @@
         <v>2014</v>
       </c>
       <c r="B115" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>174</v>
@@ -12746,7 +12731,7 @@
         <v>2014</v>
       </c>
       <c r="B116" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>175</v>
@@ -12760,13 +12745,13 @@
         <v>2014</v>
       </c>
       <c r="B117" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>181</v>
       </c>
       <c r="D117" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -12774,7 +12759,7 @@
         <v>2014</v>
       </c>
       <c r="B118" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>169</v>
@@ -12788,7 +12773,7 @@
         <v>2014</v>
       </c>
       <c r="B119" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>170</v>
@@ -12802,7 +12787,7 @@
         <v>2014</v>
       </c>
       <c r="B120" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>171</v>
@@ -12994,7 +12979,7 @@
         <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -13022,7 +13007,7 @@
         <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -13064,7 +13049,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -13078,7 +13063,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -13218,7 +13203,7 @@
         <v>282</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -13288,7 +13273,7 @@
         <v>287</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -13344,7 +13329,7 @@
         <v>291</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -13372,7 +13357,7 @@
         <v>293</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -13397,10 +13382,10 @@
         <v>79</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -13411,7 +13396,7 @@
         <v>79</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>314</v>
@@ -13425,10 +13410,10 @@
         <v>79</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -13439,10 +13424,10 @@
         <v>79</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -13453,10 +13438,10 @@
         <v>79</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -13484,7 +13469,7 @@
         <v>168</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -13526,7 +13511,7 @@
         <v>181</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -13610,7 +13595,7 @@
         <v>181</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -13666,7 +13651,7 @@
         <v>167</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -13680,7 +13665,7 @@
         <v>168</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -13694,7 +13679,7 @@
         <v>174</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -13708,7 +13693,7 @@
         <v>175</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -13722,7 +13707,7 @@
         <v>176</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -13750,7 +13735,7 @@
         <v>178</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -13764,7 +13749,7 @@
         <v>179</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -13778,7 +13763,7 @@
         <v>180</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -13792,7 +13777,7 @@
         <v>181</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -13848,7 +13833,7 @@
         <v>167</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -13876,7 +13861,7 @@
         <v>174</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -13932,7 +13917,7 @@
         <v>178</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -13946,7 +13931,7 @@
         <v>179</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -13974,7 +13959,7 @@
         <v>283</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -14002,7 +13987,7 @@
         <v>181</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -14058,7 +14043,7 @@
         <v>167</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -14072,7 +14057,7 @@
         <v>168</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -14086,7 +14071,7 @@
         <v>181</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -14142,7 +14127,7 @@
         <v>167</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -14156,7 +14141,7 @@
         <v>168</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -14170,7 +14155,7 @@
         <v>181</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -14226,7 +14211,7 @@
         <v>167</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -14240,7 +14225,7 @@
         <v>168</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -14268,7 +14253,7 @@
         <v>175</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -14310,7 +14295,7 @@
         <v>178</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -14324,7 +14309,7 @@
         <v>179</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -14352,7 +14337,7 @@
         <v>181</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -14402,13 +14387,13 @@
         <v>2016</v>
       </c>
       <c r="B113" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>167</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -14416,7 +14401,7 @@
         <v>2016</v>
       </c>
       <c r="B114" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>168</v>
@@ -14430,7 +14415,7 @@
         <v>2016</v>
       </c>
       <c r="B115" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>174</v>
@@ -14444,7 +14429,7 @@
         <v>2016</v>
       </c>
       <c r="B116" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>175</v>
@@ -14458,13 +14443,13 @@
         <v>2016</v>
       </c>
       <c r="B117" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>181</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -14472,7 +14457,7 @@
         <v>2016</v>
       </c>
       <c r="B118" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>169</v>
@@ -14486,7 +14471,7 @@
         <v>2016</v>
       </c>
       <c r="B119" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>170</v>
@@ -14500,7 +14485,7 @@
         <v>2016</v>
       </c>
       <c r="B120" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>171</v>
@@ -14691,7 +14676,7 @@
         <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -14719,7 +14704,7 @@
         <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -14761,7 +14746,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -14775,7 +14760,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -14915,7 +14900,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -14985,7 +14970,7 @@
         <v>14</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -15041,7 +15026,7 @@
         <v>18</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -15069,7 +15054,7 @@
         <v>20</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -15097,7 +15082,7 @@
         <v>22</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -15125,7 +15110,7 @@
         <v>24</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -15139,7 +15124,7 @@
         <v>25</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -15153,7 +15138,7 @@
         <v>26</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -15181,7 +15166,7 @@
         <v>2</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -15223,7 +15208,7 @@
         <v>-1</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -15307,7 +15292,7 @@
         <v>-1</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -15363,7 +15348,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -15377,7 +15362,7 @@
         <v>2</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -15391,7 +15376,7 @@
         <v>3</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -15405,7 +15390,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -15419,7 +15404,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -15447,7 +15432,7 @@
         <v>7</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -15461,7 +15446,7 @@
         <v>8</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -15475,7 +15460,7 @@
         <v>9</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -15489,7 +15474,7 @@
         <v>-1</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -15545,7 +15530,7 @@
         <v>1</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -15573,7 +15558,7 @@
         <v>3</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -15587,7 +15572,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -15643,7 +15628,7 @@
         <v>8</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -15671,7 +15656,7 @@
         <v>10</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -15699,7 +15684,7 @@
         <v>-1</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -15755,7 +15740,7 @@
         <v>1</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -15769,7 +15754,7 @@
         <v>2</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -15783,7 +15768,7 @@
         <v>-1</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -15839,7 +15824,7 @@
         <v>1</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -15853,7 +15838,7 @@
         <v>2</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -15867,7 +15852,7 @@
         <v>-1</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -15923,7 +15908,7 @@
         <v>1</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -15937,7 +15922,7 @@
         <v>2</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -15965,7 +15950,7 @@
         <v>4</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -15993,7 +15978,7 @@
         <v>6</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -16021,7 +16006,7 @@
         <v>8</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -16049,7 +16034,7 @@
         <v>-1</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -16105,7 +16090,7 @@
         <v>1</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -16161,7 +16146,7 @@
         <v>-1</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -18223,7 +18208,7 @@
   <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23002,7 +22987,7 @@
         <v>179</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -23030,7 +23015,7 @@
         <v>283</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -23100,7 +23085,7 @@
         <v>167</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -23114,7 +23099,7 @@
         <v>168</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -23170,7 +23155,7 @@
         <v>167</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -23184,7 +23169,7 @@
         <v>168</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -23240,7 +23225,7 @@
         <v>167</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -23254,7 +23239,7 @@
         <v>168</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -23324,7 +23309,7 @@
         <v>178</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -23519,8 +23504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9942FE2-02FE-0447-8EFB-7DD7FBDD6A84}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:A108"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="N82" sqref="N82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23820,7 +23805,7 @@
         <v>141</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -23848,7 +23833,7 @@
         <v>164</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -23862,7 +23847,7 @@
         <v>165</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -23876,7 +23861,7 @@
         <v>279</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -23890,7 +23875,7 @@
         <v>280</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -23904,7 +23889,7 @@
         <v>281</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -23918,7 +23903,7 @@
         <v>282</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -23932,7 +23917,7 @@
         <v>283</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -23946,7 +23931,7 @@
         <v>284</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -23960,7 +23945,7 @@
         <v>285</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -23974,7 +23959,7 @@
         <v>286</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -23988,7 +23973,7 @@
         <v>287</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -24002,7 +23987,7 @@
         <v>288</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -24016,7 +24001,7 @@
         <v>289</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -24030,7 +24015,7 @@
         <v>290</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -24044,7 +24029,7 @@
         <v>291</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -24058,7 +24043,7 @@
         <v>292</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -24072,7 +24057,7 @@
         <v>293</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -24184,7 +24169,7 @@
         <v>171</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -24254,7 +24239,7 @@
         <v>171</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -24422,7 +24407,7 @@
         <v>171</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -24436,7 +24421,7 @@
         <v>167</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>329</v>
+        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -24478,7 +24463,7 @@
         <v>175</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>330</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -24520,7 +24505,7 @@
         <v>178</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>331</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -24534,7 +24519,7 @@
         <v>179</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>332</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -24562,7 +24547,7 @@
         <v>283</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -24618,7 +24603,7 @@
         <v>171</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -24632,7 +24617,7 @@
         <v>167</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -24646,7 +24631,7 @@
         <v>168</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -24688,7 +24673,7 @@
         <v>171</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -24702,7 +24687,7 @@
         <v>167</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -24716,7 +24701,7 @@
         <v>168</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -24758,7 +24743,7 @@
         <v>171</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -24772,7 +24757,7 @@
         <v>167</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>363</v>
+        <v>417</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -24786,7 +24771,7 @@
         <v>168</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -24856,7 +24841,7 @@
         <v>178</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -24912,7 +24897,7 @@
         <v>171</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -25038,7 +25023,7 @@
         <v>171</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -26064,7 +26049,7 @@
         <v>179</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -26092,7 +26077,7 @@
         <v>283</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -26162,7 +26147,7 @@
         <v>167</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -26176,7 +26161,7 @@
         <v>168</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -26232,7 +26217,7 @@
         <v>167</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -26246,7 +26231,7 @@
         <v>168</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -26302,7 +26287,7 @@
         <v>167</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -26316,7 +26301,7 @@
         <v>168</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -26386,7 +26371,7 @@
         <v>178</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>